<commit_message>
fixed some import issues for ceu and copenhagen
</commit_message>
<xml_diff>
--- a/pilot_data/pilot_1b_copenhagen/raw_data/MB2_pilot1b_KU_CPH_participantsheet_children.xlsx
+++ b/pilot_data/pilot_1b_copenhagen/raw_data/MB2_pilot1b_KU_CPH_participantsheet_children.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galraz1/Developer/mb2-analysis/pilot_data/pilot_1b_copenhagen/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820C67FF-215E-C04F-8576-B8A1D0411C71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A708347-944D-C64F-B5FA-DA31BB5E8AC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="4600" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29980" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Variable Explanations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -204,9 +204,6 @@
     <t>KU_CPH_Southgate</t>
   </si>
   <si>
-    <t>MB2_P1b_01</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dora </t>
   </si>
   <si>
@@ -252,9 +249,6 @@
     <t>female</t>
   </si>
   <si>
-    <t>MB2_P1b_02</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -267,18 +261,9 @@
     <t>35-40</t>
   </si>
   <si>
-    <t>MB2_P1b_03</t>
-  </si>
-  <si>
     <t>had to start fast as baby got fussy, and the mother did not wear the glasses. May have also looked videos; but did not comment or otherwise interfere</t>
   </si>
   <si>
-    <t>MB2_P1b_04</t>
-  </si>
-  <si>
-    <t>MB2_P1b_05</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -511,6 +496,21 @@
   </si>
   <si>
     <t>Did caregivers report anthing else in the questionnaire?</t>
+  </si>
+  <si>
+    <t>p1b01</t>
+  </si>
+  <si>
+    <t>p1b05</t>
+  </si>
+  <si>
+    <t>p1b02</t>
+  </si>
+  <si>
+    <t>p1b03</t>
+  </si>
+  <si>
+    <t>p1b04</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -597,6 +597,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -917,9 +918,9 @@
   </sheetPr>
   <dimension ref="A1:BD970"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1011,7 +1012,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>12</v>
@@ -1147,141 +1148,141 @@
       <c r="A2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="L2" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="M2" s="7">
         <v>745</v>
       </c>
       <c r="N2" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="P2" s="11">
         <v>100</v>
       </c>
       <c r="Q2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="U2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="U2" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="V2" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="X2" s="2">
         <v>50</v>
       </c>
       <c r="Y2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="Z2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="AN2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AO2" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="AP2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AQ2" s="7">
         <v>17</v>
       </c>
       <c r="AR2" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AS2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="AT2" s="8" t="s">
-        <v>68</v>
-      </c>
       <c r="AU2" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AV2" s="8">
         <v>15</v>
@@ -1293,7 +1294,7 @@
         <v>30</v>
       </c>
       <c r="AY2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AZ2" s="2">
         <v>5</v>
@@ -1302,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="BB2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BC2" s="2">
         <v>35</v>
@@ -1313,138 +1314,138 @@
       <c r="A3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>72</v>
+      <c r="B3" s="18" t="s">
+        <v>156</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="G3" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M3" s="7">
         <v>771</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P3" s="11">
         <v>90</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R3" s="11">
         <v>10</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U3" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V3" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AE3" s="8">
         <v>13</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AG3" s="2">
         <v>9</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AJ3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AN3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AO3" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="AP3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AQ3" s="8">
         <v>20</v>
       </c>
       <c r="AR3" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AS3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU3" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="AT3" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="AU3" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="AV3" s="8">
         <v>17</v>
@@ -1465,10 +1466,10 @@
         <v>0</v>
       </c>
       <c r="BB3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BC3" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="BD3" s="2"/>
     </row>
@@ -1476,141 +1477,141 @@
       <c r="A4" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>77</v>
+      <c r="B4" s="18" t="s">
+        <v>157</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="E4" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M4" s="7">
         <v>777</v>
       </c>
       <c r="N4" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="P4" s="11">
         <v>100</v>
       </c>
       <c r="Q4" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="W4" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="R4" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="U4" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="V4" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="X4" s="2">
         <v>21</v>
       </c>
       <c r="Y4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="Z4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="AN4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AO4" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="AP4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AQ4" s="8">
         <v>13</v>
       </c>
       <c r="AR4" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AS4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT4" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="AT4" s="8" t="s">
-        <v>68</v>
-      </c>
       <c r="AU4" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AV4" s="8">
         <v>15</v>
@@ -1622,7 +1623,7 @@
         <v>40</v>
       </c>
       <c r="AY4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AZ4" s="2">
         <v>4</v>
@@ -1631,7 +1632,7 @@
         <v>0</v>
       </c>
       <c r="BB4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BC4" s="2">
         <v>40</v>
@@ -1642,138 +1643,138 @@
       <c r="A5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>79</v>
+      <c r="B5" s="18" t="s">
+        <v>158</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="E5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="G5" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M5" s="8">
         <v>776</v>
       </c>
       <c r="N5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="P5" s="11">
         <v>100</v>
       </c>
       <c r="Q5" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="R5" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="Z5" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="AA5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AH5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AI5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AJ5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AN5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AO5" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="AP5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AQ5" s="8">
         <v>12</v>
       </c>
       <c r="AR5" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AS5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT5" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="AT5" s="8" t="s">
-        <v>68</v>
-      </c>
       <c r="AU5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AV5" s="8">
         <v>17</v>
@@ -1794,7 +1795,7 @@
         <v>1</v>
       </c>
       <c r="BB5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BC5" s="2">
         <v>30</v>
@@ -1805,139 +1806,139 @@
       <c r="A6" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>80</v>
+      <c r="B6" s="18" t="s">
+        <v>155</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="E6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M6" s="7">
         <v>753</v>
       </c>
       <c r="N6" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="P6" s="11">
         <v>99</v>
       </c>
       <c r="Q6" s="16" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="R6" s="11">
         <v>1</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V6" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AH6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AI6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AJ6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AK6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AN6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AO6" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="AP6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AQ6" s="7">
         <v>15</v>
       </c>
       <c r="AR6" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AS6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT6" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="AT6" s="8" t="s">
-        <v>68</v>
-      </c>
       <c r="AU6" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AV6" s="8">
         <v>15</v>
@@ -1949,7 +1950,7 @@
         <v>50</v>
       </c>
       <c r="AY6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AZ6" s="2">
         <v>25</v>
@@ -1958,7 +1959,7 @@
         <v>6</v>
       </c>
       <c r="BB6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BC6" s="2">
         <v>36</v>
@@ -1967,7 +1968,7 @@
     </row>
     <row r="7" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -3580,16 +3581,16 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
@@ -3617,17 +3618,17 @@
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+        <v>82</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
@@ -3651,13 +3652,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -3685,13 +3686,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>91</v>
-      </c>
       <c r="D4" s="15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
@@ -3716,16 +3717,16 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -3753,13 +3754,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
@@ -3787,13 +3788,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -3821,13 +3822,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -3855,13 +3856,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -3889,13 +3890,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -3923,13 +3924,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
@@ -3954,16 +3955,16 @@
     </row>
     <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C12" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>106</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>111</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -3991,13 +3992,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -4022,16 +4023,16 @@
     </row>
     <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -4059,13 +4060,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -4093,13 +4094,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -4127,13 +4128,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -4161,13 +4162,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -4195,13 +4196,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -4229,13 +4230,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -4263,13 +4264,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C21" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>121</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>126</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -4297,13 +4298,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -4331,13 +4332,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -4365,13 +4366,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -4399,13 +4400,13 @@
         <v>22</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -4433,13 +4434,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -4467,13 +4468,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -4501,13 +4502,13 @@
         <v>25</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -4535,13 +4536,13 @@
         <v>26</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -4569,13 +4570,13 @@
         <v>27</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C30" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="15" t="s">
         <v>133</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>138</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -4603,13 +4604,13 @@
         <v>28</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -4637,13 +4638,13 @@
         <v>29</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
@@ -4671,13 +4672,13 @@
         <v>30</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
@@ -4705,13 +4706,13 @@
         <v>31</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
@@ -4739,13 +4740,13 @@
         <v>32</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E35" s="15"/>
       <c r="F35" s="15"/>
@@ -4773,13 +4774,13 @@
         <v>33</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E36" s="15"/>
       <c r="F36" s="15"/>
@@ -4807,13 +4808,13 @@
         <v>34</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
@@ -4841,13 +4842,13 @@
         <v>35</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
@@ -4875,13 +4876,13 @@
         <v>36</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
@@ -4909,13 +4910,13 @@
         <v>37</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E40" s="15"/>
       <c r="F40" s="15"/>
@@ -4943,13 +4944,13 @@
         <v>38</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E41" s="15"/>
       <c r="F41" s="15"/>
@@ -4977,13 +4978,13 @@
         <v>39</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E42" s="15"/>
       <c r="F42" s="15"/>
@@ -5011,21 +5012,21 @@
         <v>40</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E43" s="15"/>
       <c r="F43" s="15"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
       <c r="N43" s="15"/>
@@ -5045,13 +5046,13 @@
         <v>41</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E44" s="15"/>
       <c r="F44" s="15"/>
@@ -5079,13 +5080,13 @@
         <v>42</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E45" s="15"/>
       <c r="F45" s="15"/>
@@ -5113,13 +5114,13 @@
         <v>43</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
@@ -5147,13 +5148,13 @@
         <v>44</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
@@ -5181,21 +5182,21 @@
         <v>45</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E48" s="15"/>
       <c r="F48" s="15"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
       <c r="N48" s="15"/>
@@ -5215,13 +5216,13 @@
         <v>46</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E49" s="15"/>
       <c r="F49" s="15"/>
@@ -5249,13 +5250,13 @@
         <v>47</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E50" s="15"/>
       <c r="F50" s="15"/>
@@ -5283,13 +5284,13 @@
         <v>48</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E51" s="15"/>
       <c r="F51" s="15"/>
@@ -5317,13 +5318,13 @@
         <v>49</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E52" s="15"/>
       <c r="F52" s="15"/>
@@ -5351,13 +5352,13 @@
         <v>50</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E53" s="15"/>
       <c r="F53" s="15"/>
@@ -5385,13 +5386,13 @@
         <v>51</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E54" s="15"/>
       <c r="F54" s="15"/>
@@ -5419,13 +5420,13 @@
         <v>52</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="15"/>
@@ -5453,13 +5454,13 @@
         <v>53</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E56" s="15"/>
       <c r="F56" s="15"/>
@@ -5487,13 +5488,13 @@
         <v>54</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>

</xml_diff>